<commit_message>
Khung chứa giao diện của chương trình
</commit_message>
<xml_diff>
--- a/DB_QUANLYTHUVIEN.xlsx
+++ b/DB_QUANLYTHUVIEN.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thực tập nhóm_TH13\Quản lý thư viện\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thực tập nhóm_TH13\BaiTapLon\QuanLyThuVien\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Overvew" sheetId="1" r:id="rId1"/>
-    <sheet name="Tables Detail" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Tables Detail" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -2369,6 +2370,802 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="828675" y="352425"/>
+          <a:ext cx="4657725" cy="2324100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="bg2">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+        </a:gradFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2286000" y="1123950"/>
+          <a:ext cx="2447925" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2286000" y="1600200"/>
+          <a:ext cx="2447925" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1114425" y="1143000"/>
+          <a:ext cx="866775" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>UserName</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1133475" y="1609725"/>
+          <a:ext cx="866775" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Password</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>160193</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>75333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>138544</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="769793" y="3504333"/>
+          <a:ext cx="6469207" cy="4825711"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="bg2">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+        </a:gradFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>	</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>     </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>Chương</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0" baseline="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t> trìnhquản lý thư  viện</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2800" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>69273</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>374073</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1943100" y="4450773"/>
+          <a:ext cx="1478973" cy="1264227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="2400"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400"/>
+            <a:t>Nhân</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" baseline="0"/>
+            <a:t> viên</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>69273</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>568036</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4572000" y="4450773"/>
+          <a:ext cx="1482436" cy="1264227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="2400"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400"/>
+            <a:t>      Sách</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>131618</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>391391</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>103909</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1960418" y="6269182"/>
+          <a:ext cx="1478973" cy="1264227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="2400"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400"/>
+            <a:t> Độc</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" baseline="0"/>
+            <a:t> giả</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>322118</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>585354</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>103909</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4589318" y="6269182"/>
+          <a:ext cx="1482436" cy="1264227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="2000"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000"/>
+            <a:t>Hướng</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0"/>
+            <a:t> dẫn</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>160192</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>189633</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectangle 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="766328" y="10286133"/>
+          <a:ext cx="12759171" cy="7551594"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="bg2">
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="bg2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+        </a:gradFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>	</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2800" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2634,7 +3431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
@@ -2650,9 +3447,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A51" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T47" sqref="T47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>

</xml_diff>